<commit_message>
Updates to the inflation analysis
</commit_message>
<xml_diff>
--- a/report_publication_dates/FSR_dates.xlsx
+++ b/report_publication_dates/FSR_dates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f0f9501e142f3e28/LSE Data Analytics/Employer Project/Employer Project files/group-project/report_publication_dates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_364663355C82C8D5AE678C0F5507EA1E67FF6D35" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73AD5379-B9E9-4354-A147-14E1A703AC5E}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_364663355C82C8D5AE678C0F5507EA1E67FF6D35" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EACE246-CDD1-42FB-918C-4EC1963F3174}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,10 +17,6 @@
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -69,15 +65,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -93,6 +90,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -298,8 +299,8 @@
   </sheetPr>
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A52" sqref="A1:A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -309,264 +310,264 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1">
+      <c r="A1" s="3">
         <v>35490</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="A2" s="3">
         <v>35704</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="A3" s="3">
         <v>35916</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="A4" s="3">
         <v>36100</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5" s="4">
         <v>36312</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6" s="4">
         <v>36465</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="A7" s="4">
         <v>36678</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="A8" s="4">
         <v>36861</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="A9" s="4">
         <v>37043</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="A10" s="4">
         <v>37226</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="A11" s="4">
         <v>37408</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="A12" s="4">
         <v>37591</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+      <c r="A13" s="4">
         <v>37773</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+      <c r="A14" s="4">
         <v>37956</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+      <c r="A15" s="4">
         <v>38139</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
+      <c r="A16" s="4">
         <v>38322</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
+      <c r="A17" s="4">
         <v>38504</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
+      <c r="A18" s="4">
         <v>38687</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
+      <c r="A19" s="4">
         <v>38899</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
+      <c r="A20" s="4">
         <v>39173</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
+      <c r="A21" s="4">
         <v>39356</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
+      <c r="A22" s="4">
         <v>39569</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
+      <c r="A23" s="4">
         <v>39722</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
+      <c r="A24" s="4">
         <v>39965</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
+      <c r="A25" s="4">
         <v>40148</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
+      <c r="A26" s="4">
         <v>40330</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
+      <c r="A27" s="4">
         <v>40513</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
+      <c r="A28" s="4">
         <v>40695</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
+      <c r="A29" s="4">
         <v>40878</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
+      <c r="A30" s="4">
         <v>41061</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
+      <c r="A31" s="4">
         <v>41214</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
+      <c r="A32" s="4">
         <v>41426</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="3">
+      <c r="A33" s="4">
         <v>41579</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3">
+      <c r="A34" s="4">
         <v>41791</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3">
+      <c r="A35" s="4">
         <v>41974</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3">
+      <c r="A36" s="4">
         <v>42186</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
+      <c r="A37" s="4">
         <v>42339</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3">
+      <c r="A38" s="4">
         <v>42552</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3">
+      <c r="A39" s="4">
         <v>42675</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3">
+      <c r="A40" s="4">
         <v>42887</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3">
+      <c r="A41" s="4">
         <v>43040</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="3">
+      <c r="A42" s="4">
         <v>43252</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3">
+      <c r="A43" s="4">
         <v>43405</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="3">
+      <c r="A44" s="4">
         <v>43647</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="3">
+      <c r="A45" s="4">
         <v>43800</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="3">
+      <c r="A46" s="4">
         <v>43952</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="3">
+      <c r="A47" s="4">
         <v>44044</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="3">
+      <c r="A48" s="4">
         <v>44166</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="3">
+      <c r="A49" s="4">
         <v>44378</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="3">
+      <c r="A50" s="4">
         <v>44531</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="3">
+      <c r="A51" s="4">
         <v>44743</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="3">
+      <c r="A52" s="4">
         <v>44896</v>
       </c>
     </row>

</xml_diff>